<commit_message>
Updated with Donation Scripts
</commit_message>
<xml_diff>
--- a/DynamicUsgbc.xlsx
+++ b/DynamicUsgbc.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Desktop\NEW USGBC\DynamicUsgbc\DynamicUsgbc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CommunityRegistration" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="205">
   <si>
     <t>CommunityName</t>
   </si>
@@ -612,9 +612,6 @@
     <t>$6000.00</t>
   </si>
   <si>
-    <t>$35.00</t>
-  </si>
-  <si>
     <t>GROUND HOME DELIVERY</t>
   </si>
   <si>
@@ -673,7 +670,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,21 +1055,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="31.1796875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="23.81640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.78515625" collapsed="true"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.1796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="31.1796875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7265625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.81640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -1175,22 +1172,22 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" t="s">
         <v>198</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>200</v>
-      </c>
-      <c r="H2" t="s">
-        <v>201</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1202,7 +1199,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O2" t="s">
         <v>13</v>
@@ -1223,7 +1220,7 @@
         <v>21</v>
       </c>
       <c r="U2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="V2" t="s">
         <v>24</v>
@@ -1262,18 +1259,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="31.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="15.54296875" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="13.26953125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -1370,28 +1367,28 @@
         <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M2" t="s">
         <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O2" t="s">
         <v>158</v>
       </c>
       <c r="P2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q2" t="s">
         <v>42</v>
       </c>
       <c r="R2" t="s">
+        <v>200</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>27</v>
@@ -1412,25 +1409,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="1" max="1" width="31.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -1503,28 +1500,28 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2" t="s">
         <v>198</v>
-      </c>
-      <c r="I2" t="s">
-        <v>199</v>
       </c>
       <c r="J2" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L2" t="s">
         <v>200</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="N2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1536,18 +1533,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.26953125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1602,25 +1601,25 @@
         <v>47</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" t="s">
         <v>198</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>199</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>200</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="L2" t="s">
         <v>50</v>
@@ -1644,11 +1643,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1694,7 +1693,7 @@
         <v>99</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
@@ -1722,14 +1721,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1787,19 +1786,19 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" t="s">
         <v>198</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>199</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>200</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1817,19 +1816,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.6328125" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="18.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="22.54296875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="33" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
@@ -1917,34 +1916,34 @@
         <v>161</v>
       </c>
       <c r="E2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" t="s">
         <v>198</v>
       </c>
-      <c r="F2" t="s">
-        <v>199</v>
-      </c>
       <c r="G2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H2" t="s">
         <v>162</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" t="s">
         <v>200</v>
-      </c>
-      <c r="J2" t="s">
-        <v>201</v>
       </c>
       <c r="K2" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
@@ -1990,10 +1989,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.54296875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2109,14 +2108,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="35.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="37.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.7265625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.36328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="41.453125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.26953125" collapsed="true"/>
+    <col min="1" max="2" width="35.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2183,10 +2182,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="1" max="1" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2232,26 +2231,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.7265625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.90625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="23.26953125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
+    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.81640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23.26953125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.26953125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
@@ -2363,31 +2362,31 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" t="s">
         <v>198</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>200</v>
-      </c>
-      <c r="H2" t="s">
-        <v>201</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K2" t="s">
         <v>103</v>
       </c>
       <c r="L2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>106</v>
@@ -2405,7 +2404,7 @@
         <v>112</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T2" t="s">
         <v>142</v>
@@ -2426,7 +2425,7 @@
         <v>151</v>
       </c>
       <c r="Z2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AA2" t="s">
         <v>184</v>

</xml_diff>

<commit_message>
Scripts to verify the modified details from payment page has updated
</commit_message>
<xml_diff>
--- a/DynamicUsgbc.xlsx
+++ b/DynamicUsgbc.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Desktop\NEW USGBC\DynamicUsgbc\DynamicUsgbc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CommunityRegistration" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="206">
   <si>
     <t>CommunityName</t>
   </si>
@@ -352,12 +352,6 @@
   </si>
   <si>
     <t>Website</t>
-  </si>
-  <si>
-    <t>www.groupten.com</t>
-  </si>
-  <si>
-    <t>info@groupten.com</t>
   </si>
   <si>
     <t>Real Estate</t>
@@ -612,58 +606,64 @@
     <t>$6000.00</t>
   </si>
   <si>
+    <t>Test Organization 675774</t>
+  </si>
+  <si>
+    <t>Annual Partnerships</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>$166.97</t>
+  </si>
+  <si>
+    <t>2019-11-10</t>
+  </si>
+  <si>
+    <t>725 chestnut st</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>erie</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>16507</t>
+  </si>
+  <si>
+    <t>gupta@gmail.com</t>
+  </si>
+  <si>
+    <t>$75.00</t>
+  </si>
+  <si>
+    <t>EditEmail</t>
+  </si>
+  <si>
+    <t>mallik@gmail.com</t>
+  </si>
+  <si>
+    <t>www.promantus.com</t>
+  </si>
+  <si>
+    <t>info@mallik.com</t>
+  </si>
+  <si>
+    <t>arjun@gmail.com</t>
+  </si>
+  <si>
+    <t>EditTerm</t>
+  </si>
+  <si>
+    <t>Test Organization 598892</t>
+  </si>
+  <si>
     <t>GROUND HOME DELIVERY</t>
-  </si>
-  <si>
-    <t>SILVER</t>
-  </si>
-  <si>
-    <t>$1500</t>
-  </si>
-  <si>
-    <t>Test Organization 675774</t>
-  </si>
-  <si>
-    <t>Annual Partnerships</t>
-  </si>
-  <si>
-    <t>$0.00</t>
-  </si>
-  <si>
-    <t>$166.97</t>
-  </si>
-  <si>
-    <t>Test Organization 611140</t>
-  </si>
-  <si>
-    <t>2019-11-10</t>
-  </si>
-  <si>
-    <t>725 chestnut st</t>
-  </si>
-  <si>
-    <t>west</t>
-  </si>
-  <si>
-    <t>erie</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>16507</t>
-  </si>
-  <si>
-    <t>gupta@gmail.com</t>
-  </si>
-  <si>
-    <t>mike@gmail.com</t>
-  </si>
-  <si>
-    <t>$75.00</t>
-  </si>
-  <si>
-    <t>Test Organization 482335</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,6 +703,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -725,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -735,6 +741,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1052,27 +1059,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="31.1796875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="23.81640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.1796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="31.1796875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7265625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.81640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -1140,25 +1147,25 @@
         <v>38</v>
       </c>
       <c r="V1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" t="s">
+        <v>138</v>
+      </c>
+      <c r="X1" t="s">
         <v>139</v>
       </c>
-      <c r="W1" t="s">
-        <v>140</v>
-      </c>
-      <c r="X1" t="s">
-        <v>141</v>
-      </c>
       <c r="Y1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z1" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>146</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>148</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
@@ -1175,22 +1182,22 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1202,7 +1209,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="O2" t="s">
         <v>13</v>
@@ -1223,28 +1230,28 @@
         <v>21</v>
       </c>
       <c r="U2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="V2" t="s">
         <v>24</v>
       </c>
       <c r="W2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y2" t="s">
         <v>143</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>145</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" t="s">
         <v>149</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1262,23 +1269,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="31.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="15.54296875" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="13.26953125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
         <v>51</v>
@@ -1287,7 +1294,7 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E1" t="s">
         <v>43</v>
@@ -1308,19 +1315,19 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
@@ -1349,16 +1356,16 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I2" t="s">
         <v>40</v>
@@ -1367,31 +1374,31 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="M2" t="s">
         <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="O2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q2" t="s">
         <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>27</v>
@@ -1418,24 +1425,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="1" max="1" width="31.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1482,7 +1489,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -1491,10 +1498,10 @@
         <v>72</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>40</v>
@@ -1503,28 +1510,28 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="J2" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="N2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="O2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1536,25 +1543,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.08984375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.26953125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
         <v>43</v>
@@ -1592,7 +1599,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -1604,25 +1611,25 @@
         <v>47</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="I2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="L2" t="s">
         <v>50</v>
@@ -1641,16 +1648,16 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1658,10 +1665,10 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
         <v>96</v>
@@ -1676,7 +1683,7 @@
         <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1684,7 +1691,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1696,13 +1703,13 @@
         <v>99</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1724,14 +1731,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1789,19 +1796,19 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="I2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1813,25 +1820,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.6328125" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="18.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="22.54296875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="33" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
@@ -1845,19 +1852,19 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -1881,7 +1888,7 @@
         <v>55</v>
       </c>
       <c r="P1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q1" t="s">
         <v>56</v>
@@ -1890,19 +1897,19 @@
         <v>57</v>
       </c>
       <c r="S1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="T1" t="s">
         <v>70</v>
       </c>
       <c r="U1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" t="s">
         <v>131</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>133</v>
-      </c>
-      <c r="W1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
@@ -1916,43 +1923,43 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K2" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M2" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="N2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q2" t="s">
         <v>26</v>
@@ -1961,19 +1968,19 @@
         <v>67</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" t="s">
         <v>134</v>
-      </c>
-      <c r="W2" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1992,10 +1999,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.54296875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2111,60 +2118,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="35.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="37.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.7265625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.36328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="41.453125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.26953125" collapsed="true"/>
+    <col min="1" max="2" width="35.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" t="s">
         <v>121</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2185,10 +2192,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="1" max="1" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2213,7 +2220,7 @@
         <v>99</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -2226,37 +2233,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.7265625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.890625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.921875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="23.26953125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.78515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
+    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.81640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23.26953125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.90625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="14.36328125" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.08984375" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -2291,7 +2305,7 @@
         <v>102</v>
       </c>
       <c r="L1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M1" t="s">
         <v>104</v>
@@ -2303,55 +2317,61 @@
         <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Q1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" t="s">
         <v>109</v>
-      </c>
-      <c r="R1" t="s">
-        <v>111</v>
       </c>
       <c r="S1" t="s">
         <v>38</v>
       </c>
       <c r="T1" t="s">
+        <v>173</v>
+      </c>
+      <c r="U1" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" t="s">
         <v>175</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>176</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>177</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>178</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>179</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD1" t="s">
         <v>180</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
         <v>181</v>
       </c>
-      <c r="AA1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2365,92 +2385,100 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2" t="s">
+        <v>204</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K2" t="s">
+      <c r="P2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="T2" t="s">
+        <v>140</v>
+      </c>
+      <c r="U2" t="s">
+        <v>141</v>
+      </c>
+      <c r="V2" t="s">
+        <v>143</v>
+      </c>
+      <c r="W2" t="s">
+        <v>145</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" t="s">
         <v>103</v>
-      </c>
-      <c r="L2" t="s">
-        <v>189</v>
-      </c>
-      <c r="M2" t="s">
-        <v>205</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="P2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>110</v>
-      </c>
-      <c r="R2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="T2" t="s">
-        <v>142</v>
-      </c>
-      <c r="U2" t="s">
-        <v>143</v>
-      </c>
-      <c r="V2" t="s">
-        <v>145</v>
-      </c>
-      <c r="W2" t="s">
-        <v>147</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
     <hyperlink ref="O2" r:id="rId2"/>
+    <hyperlink ref="AF2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exam and Sponsor edit scripts
</commit_message>
<xml_diff>
--- a/DynamicUsgbc.xlsx
+++ b/DynamicUsgbc.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Desktop\NEW USGBC\DynamicUsgbc\DynamicUsgbc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="CommunityRegistration" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="206">
   <si>
     <t>CommunityName</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Manager</t>
-  </si>
-  <si>
-    <t>Promentus</t>
   </si>
   <si>
     <t>11</t>
@@ -612,9 +609,6 @@
     <t>Annual Partnerships</t>
   </si>
   <si>
-    <t>$0.00</t>
-  </si>
-  <si>
     <t>$166.97</t>
   </si>
   <si>
@@ -664,6 +658,12 @@
   </si>
   <si>
     <t>GROUND HOME DELIVERY</t>
+  </si>
+  <si>
+    <t>$200.00</t>
+  </si>
+  <si>
+    <t>$1000.00</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,21 +1065,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.1796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="31.1796875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.1796875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.81640625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.7265625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.26953125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.81640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="21.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.81640625" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="31.1796875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.81640625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="23.81640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -1147,25 +1147,25 @@
         <v>38</v>
       </c>
       <c r="V1" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1" t="s">
         <v>137</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>138</v>
       </c>
-      <c r="X1" t="s">
-        <v>139</v>
-      </c>
       <c r="Y1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AA1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
@@ -1182,22 +1182,22 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" t="s">
         <v>191</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>192</v>
-      </c>
-      <c r="G2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" t="s">
-        <v>194</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1209,13 +1209,13 @@
         <v>26</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
         <v>28</v>
@@ -1230,28 +1230,28 @@
         <v>21</v>
       </c>
       <c r="U2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="V2" t="s">
         <v>24</v>
       </c>
       <c r="W2" t="s">
+        <v>139</v>
+      </c>
+      <c r="X2" t="s">
         <v>140</v>
       </c>
-      <c r="X2" t="s">
-        <v>141</v>
-      </c>
       <c r="Y2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1263,29 +1263,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="12.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="15.54296875" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="13.26953125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.6328125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
         <v>51</v>
@@ -1294,7 +1295,7 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
         <v>43</v>
@@ -1315,19 +1316,19 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
@@ -1356,16 +1357,16 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="I2" t="s">
         <v>40</v>
@@ -1374,31 +1375,31 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M2" t="s">
         <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="O2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q2" t="s">
         <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>27</v>
@@ -1407,7 +1408,7 @@
         <v>60</v>
       </c>
       <c r="V2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1417,32 +1418,34 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26953125" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.453125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="16.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.1796875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.78515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="18.26953125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="13.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1451,10 +1454,10 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -1484,24 +1487,30 @@
         <v>38</v>
       </c>
       <c r="O1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>40</v>
@@ -1510,28 +1519,34 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J2" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="L2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="N2" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="O2" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="P2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1549,19 +1564,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.26953125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.08984375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.1796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.08984375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
         <v>43</v>
@@ -1599,7 +1614,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -1611,25 +1626,25 @@
         <v>47</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2" t="s">
         <v>191</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>192</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="J2" t="s">
-        <v>194</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="L2" t="s">
         <v>50</v>
@@ -1653,11 +1668,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.26953125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.453125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1665,16 +1680,16 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" t="s">
-        <v>124</v>
-      </c>
       <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
       </c>
       <c r="F1" t="s">
         <v>28</v>
@@ -1683,7 +1698,7 @@
         <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1691,25 +1706,25 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
-        <v>99</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1731,14 +1746,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.81640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1784,31 +1799,31 @@
         <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2" t="s">
         <v>191</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>192</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="J2" t="s">
-        <v>194</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1820,25 +1835,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="18.1796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="22.54296875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="11.453125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.54296875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="33" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.54296875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="18" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" width="18.1796875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.6328125" collapsed="true"/>
+    <col min="15" max="16" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="16.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
@@ -1852,19 +1867,19 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -1879,7 +1894,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>38</v>
@@ -1888,7 +1903,7 @@
         <v>55</v>
       </c>
       <c r="P1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q1" t="s">
         <v>56</v>
@@ -1897,24 +1912,24 @@
         <v>57</v>
       </c>
       <c r="S1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -1923,64 +1938,64 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" t="s">
         <v>159</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>192</v>
-      </c>
-      <c r="G2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="J2" t="s">
-        <v>194</v>
       </c>
       <c r="K2" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q2" t="s">
         <v>26</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1999,108 +2014,108 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
         <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
         <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
         <v>89</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2118,60 +2133,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="35.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.26953125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.26953125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="35.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="37.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="43.7265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.36328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.453125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.26953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>117</v>
-      </c>
-      <c r="G1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G2" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2192,18 +2207,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
         <v>96</v>
-      </c>
-      <c r="B1" t="s">
-        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
@@ -2214,13 +2229,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -2241,41 +2256,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.26953125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.26953125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.81640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.81640625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="23.26953125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.1796875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="22.81640625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.1796875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.90625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.36328125" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.08984375" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="16.26953125" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.81640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.26953125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.90625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="22.81640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="23.26953125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.1796875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="22.81640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="14.36328125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="16.08984375" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="13.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2302,78 +2317,78 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" t="s">
         <v>104</v>
-      </c>
-      <c r="N1" t="s">
-        <v>105</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S1" t="s">
         <v>38</v>
       </c>
       <c r="T1" t="s">
+        <v>172</v>
+      </c>
+      <c r="U1" t="s">
         <v>173</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>174</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>175</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>176</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>177</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>178</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD1" t="s">
         <v>179</v>
       </c>
-      <c r="AA1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>180</v>
       </c>
-      <c r="AE1" t="s">
-        <v>181</v>
-      </c>
       <c r="AF1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AG1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -2385,91 +2400,91 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" t="s">
         <v>191</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>192</v>
-      </c>
-      <c r="G2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" t="s">
-        <v>194</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="T2" t="s">
+        <v>139</v>
+      </c>
+      <c r="U2" t="s">
+        <v>140</v>
+      </c>
+      <c r="V2" t="s">
+        <v>142</v>
+      </c>
+      <c r="W2" t="s">
+        <v>144</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD2" t="s">
         <v>170</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="M2" t="s">
-        <v>204</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="P2" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>108</v>
-      </c>
-      <c r="R2" t="s">
-        <v>110</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="T2" t="s">
-        <v>140</v>
-      </c>
-      <c r="U2" t="s">
-        <v>141</v>
-      </c>
-      <c r="V2" t="s">
-        <v>143</v>
-      </c>
-      <c r="W2" t="s">
-        <v>145</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>186</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>171</v>
       </c>
-      <c r="AE2" t="s">
-        <v>172</v>
-      </c>
       <c r="AF2" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AG2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Donation scripts with edit
</commit_message>
<xml_diff>
--- a/DynamicUsgbc.xlsx
+++ b/DynamicUsgbc.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Desktop\NEW USGBC\DynamicUsgbc\DynamicUsgbc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3960" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CommunityRegistration" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="206">
   <si>
     <t>CommunityName</t>
   </si>
@@ -673,7 +673,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,21 +1065,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="31.1796875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="23.81640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.1796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="31.1796875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7265625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.81640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -1269,19 +1269,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.6328125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="31.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="15.54296875" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="13.26953125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.6328125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -1420,27 +1420,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.78515625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="18.26953125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="1" max="1" width="31.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.26953125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
@@ -1558,20 +1558,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.08984375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.26953125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1668,11 +1669,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1746,14 +1747,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1841,19 +1842,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="20.1796875" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.6328125" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="18.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="20.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="22.54296875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="33" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
@@ -2014,10 +2015,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.54296875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2133,14 +2134,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="35.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="37.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.7265625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.36328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="41.453125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.26953125" collapsed="true"/>
+    <col min="1" max="2" width="35.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2207,10 +2208,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="1" max="1" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2256,33 +2257,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.7265625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.90625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="23.26953125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="11.90625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="14.36328125" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="16.08984375" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.26953125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.81640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23.26953125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.1796875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.90625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="14.36328125" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.08984375" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">

</xml_diff>